<commit_message>
Change the formatting for numeric columns.
</commit_message>
<xml_diff>
--- a/data/Table6.7.xlsx
+++ b/data/Table6.7.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Applied-Multivariate-Statistical-Analysis-Solutions\Applied-Multivariate-Statistical-Analysis-Solutions\Applied-Multivariate-Statistical-Analysis-Solutions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7874C193-D0AE-4606-BF62-B917FDBB1EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5694BC6-9DDF-43C4-A671-5F74EF1227CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{55D62A12-6AA2-41AF-BA97-6C890FA76C26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{55D62A12-6AA2-41AF-BA97-6C890FA76C26}"/>
   </bookViews>
   <sheets>
     <sheet name="T6-7" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -35,6 +48,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="19">
     <font>
       <sz val="11"/>
@@ -519,9 +536,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -915,10 +934,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>7.5129999999999999</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>74</v>
       </c>
       <c r="C2">
@@ -926,10 +945,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>5.032</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>69.5</v>
       </c>
       <c r="C3">
@@ -937,10 +956,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>5.867</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>72</v>
       </c>
       <c r="C4">
@@ -948,10 +967,10 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>11.087999999999999</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>80</v>
       </c>
       <c r="C5">
@@ -959,10 +978,10 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>2.419</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>56</v>
       </c>
       <c r="C6">
@@ -970,10 +989,10 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>13.61</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>94</v>
       </c>
       <c r="C7">
@@ -981,10 +1000,10 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>18.247</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>95.5</v>
       </c>
       <c r="C8">
@@ -992,10 +1011,10 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>16.832000000000001</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>99.5</v>
       </c>
       <c r="C9">
@@ -1003,10 +1022,10 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>15.91</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>97</v>
       </c>
       <c r="C10">
@@ -1014,10 +1033,10 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>17.035</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>90.5</v>
       </c>
       <c r="C11">
@@ -1025,10 +1044,10 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>16.526</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>91</v>
       </c>
       <c r="C12">
@@ -1036,10 +1055,10 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>4.53</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>67</v>
       </c>
       <c r="C13">
@@ -1047,10 +1066,10 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>7.23</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>75</v>
       </c>
       <c r="C14">
@@ -1058,10 +1077,10 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>5.2</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>69.5</v>
       </c>
       <c r="C15">
@@ -1069,10 +1088,10 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>13.45</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>91.5</v>
       </c>
       <c r="C16">
@@ -1080,10 +1099,10 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>14.08</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>91</v>
       </c>
       <c r="C17">
@@ -1091,10 +1110,10 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>14.664999999999999</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>90</v>
       </c>
       <c r="C18">
@@ -1102,10 +1121,10 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19">
+      <c r="A19" s="2">
         <v>6.0919999999999996</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>73</v>
       </c>
       <c r="C19">
@@ -1113,10 +1132,10 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20">
+      <c r="A20" s="2">
         <v>5.2640000000000002</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>69.5</v>
       </c>
       <c r="C20">
@@ -1124,10 +1143,10 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21">
+      <c r="A21" s="2">
         <v>16.902000000000001</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <v>94</v>
       </c>
       <c r="C21">
@@ -1135,10 +1154,10 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22">
+      <c r="A22" s="2">
         <v>13.911</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>77</v>
       </c>
       <c r="C22">
@@ -1146,10 +1165,10 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23">
+      <c r="A23" s="2">
         <v>5.2359999999999998</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>62</v>
       </c>
       <c r="C23">
@@ -1157,10 +1176,10 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24">
+      <c r="A24" s="2">
         <v>37.331000000000003</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="3">
         <v>108</v>
       </c>
       <c r="C24">
@@ -1168,10 +1187,10 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25">
+      <c r="A25" s="2">
         <v>41.780999999999999</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>115</v>
       </c>
       <c r="C25">
@@ -1179,10 +1198,10 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26">
+      <c r="A26" s="2">
         <v>31.995000000000001</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="3">
         <v>106</v>
       </c>
       <c r="C26">
@@ -1190,10 +1209,10 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27">
+      <c r="A27" s="2">
         <v>3.9620000000000002</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="3">
         <v>56</v>
       </c>
       <c r="C27">
@@ -1201,10 +1220,10 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28">
+      <c r="A28" s="2">
         <v>4.367</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="3">
         <v>60.5</v>
       </c>
       <c r="C28">
@@ -1212,10 +1231,10 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29">
+      <c r="A29" s="2">
         <v>3.048</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="3">
         <v>52</v>
       </c>
       <c r="C29">
@@ -1223,10 +1242,10 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30">
+      <c r="A30" s="2">
         <v>4.8380000000000001</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="3">
         <v>60</v>
       </c>
       <c r="C30">
@@ -1234,10 +1253,10 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31">
+      <c r="A31" s="2">
         <v>6.5250000000000004</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="3">
         <v>64</v>
       </c>
       <c r="C31">
@@ -1245,10 +1264,10 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32">
+      <c r="A32" s="2">
         <v>22.61</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="3">
         <v>96</v>
       </c>
       <c r="C32">
@@ -1256,10 +1275,10 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33">
+      <c r="A33" s="2">
         <v>13.342000000000001</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="3">
         <v>79.5</v>
       </c>
       <c r="C33">
@@ -1267,10 +1286,10 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34">
+      <c r="A34" s="2">
         <v>4.109</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="3">
         <v>55.5</v>
       </c>
       <c r="C34">
@@ -1278,10 +1297,10 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35">
+      <c r="A35" s="2">
         <v>12.369</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="3">
         <v>75</v>
       </c>
       <c r="C35">
@@ -1289,10 +1308,10 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36">
+      <c r="A36" s="2">
         <v>7.12</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="3">
         <v>64.5</v>
       </c>
       <c r="C36">
@@ -1300,10 +1319,10 @@
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37">
+      <c r="A37" s="2">
         <v>21.077000000000002</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="3">
         <v>87.5</v>
       </c>
       <c r="C37">
@@ -1311,10 +1330,10 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38">
+      <c r="A38" s="2">
         <v>42.988999999999997</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="3">
         <v>109</v>
       </c>
       <c r="C38">
@@ -1322,10 +1341,10 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39">
+      <c r="A39" s="2">
         <v>27.201000000000001</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="3">
         <v>96</v>
       </c>
       <c r="C39">
@@ -1333,10 +1352,10 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40">
+      <c r="A40" s="2">
         <v>38.901000000000003</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="3">
         <v>111</v>
       </c>
       <c r="C40">
@@ -1344,10 +1363,10 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41">
+      <c r="A41" s="2">
         <v>19.747</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="3">
         <v>84.5</v>
       </c>
       <c r="C41">
@@ -1355,10 +1374,10 @@
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42">
+      <c r="A42" s="2">
         <v>14.666</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="3">
         <v>80</v>
       </c>
       <c r="C42">
@@ -1366,10 +1385,10 @@
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43">
+      <c r="A43" s="2">
         <v>4.79</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="3">
         <v>62</v>
       </c>
       <c r="C43">
@@ -1377,10 +1396,10 @@
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44">
+      <c r="A44" s="2">
         <v>5.0199999999999996</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="3">
         <v>61.5</v>
       </c>
       <c r="C44">
@@ -1388,10 +1407,10 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45">
+      <c r="A45" s="2">
         <v>5.22</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="3">
         <v>62</v>
       </c>
       <c r="C45">
@@ -1399,10 +1418,10 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46">
+      <c r="A46" s="2">
         <v>5.69</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="3">
         <v>64</v>
       </c>
       <c r="C46">
@@ -1410,10 +1429,10 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47">
+      <c r="A47" s="2">
         <v>6.7629999999999999</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="3">
         <v>63</v>
       </c>
       <c r="C47">
@@ -1421,10 +1440,10 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48">
+      <c r="A48" s="2">
         <v>9.9770000000000003</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="3">
         <v>71</v>
       </c>
       <c r="C48">
@@ -1432,10 +1451,10 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49">
+      <c r="A49" s="2">
         <v>8.8309999999999995</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="3">
         <v>69.5</v>
       </c>
       <c r="C49">
@@ -1443,10 +1462,10 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50">
+      <c r="A50" s="2">
         <v>9.4930000000000003</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="3">
         <v>67.5</v>
       </c>
       <c r="C50">
@@ -1454,10 +1473,10 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51">
+      <c r="A51" s="2">
         <v>7.8109999999999999</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="3">
         <v>66</v>
       </c>
       <c r="C51">
@@ -1465,10 +1484,10 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52">
+      <c r="A52" s="2">
         <v>6.6849999999999996</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="3">
         <v>64.5</v>
       </c>
       <c r="C52">
@@ -1476,10 +1495,10 @@
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53">
+      <c r="A53" s="2">
         <v>11.98</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="3">
         <v>79</v>
       </c>
       <c r="C53">
@@ -1487,10 +1506,10 @@
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54">
+      <c r="A54" s="2">
         <v>16.52</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="3">
         <v>84</v>
       </c>
       <c r="C54">
@@ -1498,10 +1517,10 @@
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55">
+      <c r="A55" s="2">
         <v>13.63</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="3">
         <v>81</v>
       </c>
       <c r="C55">
@@ -1509,10 +1528,10 @@
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56">
+      <c r="A56" s="2">
         <v>13.7</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="3">
         <v>82.5</v>
       </c>
       <c r="C56">
@@ -1520,10 +1539,10 @@
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57">
+      <c r="A57" s="2">
         <v>10.35</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="3">
         <v>74</v>
       </c>
       <c r="C57">
@@ -1531,10 +1550,10 @@
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58">
+      <c r="A58" s="2">
         <v>7.9</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="3">
         <v>68.5</v>
       </c>
       <c r="C58">
@@ -1542,10 +1561,10 @@
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59">
+      <c r="A59" s="2">
         <v>9.1029999999999998</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="3">
         <v>70</v>
       </c>
       <c r="C59">
@@ -1553,10 +1572,10 @@
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60">
+      <c r="A60" s="2">
         <v>13.215999999999999</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="3">
         <v>77.5</v>
       </c>
       <c r="C60">
@@ -1564,10 +1583,10 @@
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61">
+      <c r="A61" s="2">
         <v>9.7870000000000008</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="3">
         <v>70</v>
       </c>
       <c r="C61">

</xml_diff>